<commit_message>
fix follow / unfollow
</commit_message>
<xml_diff>
--- a/docs/atyichu revision.xlsx
+++ b/docs/atyichu revision.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="store" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="wechat" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="62">
   <si>
     <t xml:space="preserve">Page</t>
   </si>
@@ -110,6 +111,102 @@
   </si>
   <si>
     <t xml:space="preserve">Update an article</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Photo lists (newest, etc)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Square avatars for store, circle avatars for visitors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Follow / unfollow (because of article description)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Comment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Article</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Similar photos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Photo at same location ( it is actually a photo of the one store, not one location)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Photo from the store</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Like / dislike</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Store location</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Photo location, looks like works, but not from original</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sharing a photo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Photo detail article</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bad template</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Edit  a photo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">My groups</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Delete</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Set private / public</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create a group</t>
+  </si>
+  <si>
+    <t xml:space="preserve">add collaborator </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Edi a group</t>
+  </si>
+  <si>
+    <t xml:space="preserve">My group photos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">broken template, fix it</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Notification</t>
+  </si>
+  <si>
+    <t xml:space="preserve">looks like it works, has bad design</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Me</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Update a profile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sync profile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Change password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not checked</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Logout</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Connect weixin account / not displays as expected, not checked</t>
   </si>
 </sst>
 </file>
@@ -141,7 +238,7 @@
       <family val="0"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -152,6 +249,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFF3333"/>
         <bgColor rgb="FFFF6600"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF99"/>
+        <bgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
   </fills>
@@ -189,12 +292,20 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -277,8 +388,8 @@
   </sheetPr>
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B24" activeCellId="0" sqref="B24"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B31" activeCellId="0" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -463,8 +574,8 @@
       <c r="A22" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="C22" s="1" t="s">
-        <v>10</v>
+      <c r="C22" s="0" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -500,4 +611,286 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Обычный"&amp;12Страница &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C29"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C20" activeCellId="0" sqref="C20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.030612244898"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="79.7551020408163"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B20" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B22" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B26" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="C26" s="0" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B27" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B28" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="C28" s="0" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B29" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="C29" s="0" t="s">
+        <v>59</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Обычный"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Обычный"&amp;12Страница &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>